<commit_message>
increase test coverage of import by triggering more cases
and make failure reporting more graceful by unwrapping ordered dicts,
since 'unittest' doesn't make line-by-line diffs for them.
</commit_message>
<xml_diff>
--- a/tests/fixtures/MAGENTA_01.xlsx
+++ b/tests/fixtures/MAGENTA_01.xlsx
@@ -1067,7 +1067,7 @@
     <t>Aarhus Enhed</t>
   </si>
   <si>
-    <t>Rådhuspladsen 2</t>
+    <t>Rådhuspladsen</t>
   </si>
   <si>
     <t>01e479c4-66ef-42aa-877e-15f0512f792c</t>
@@ -2544,9 +2544,7 @@
       <c r="I4" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="J4" t="s" s="7">
-        <v>7</v>
-      </c>
+      <c r="J4" s="7"/>
       <c r="K4" t="s" s="7">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
consolidate class support and increase test coverage
</commit_message>
<xml_diff>
--- a/tests/fixtures/MAGENTA_01.xlsx
+++ b/tests/fixtures/MAGENTA_01.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="362">
   <si>
     <t>operation</t>
   </si>
@@ -1104,25 +1104,15 @@
   </si>
   <si>
     <t>København K</t>
-  </si>
-  <si>
-    <t>3cd8be77-043c-4044-a9c1-8e4261fd7da6</t>
-  </si>
-  <si>
-    <t>Ikke eksisterende</t>
-  </si>
-  <si>
-    <t>Inaktiv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="60" formatCode="dd/mm/yyyy hh:mm"/>
+    <numFmt numFmtId="59" formatCode="dd/mm/yyyy hh:mm"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1141,7 +1131,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1154,8 +1144,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1208,13 +1204,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1224,37 +1307,58 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1275,19 +1379,19 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1310,6 +1414,8 @@
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1447,13 +1553,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -1552,10 +1652,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1810,13 +1910,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -2129,10 +2223,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2383,7 +2477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2553,6 +2647,96 @@
       </c>
       <c r="M4" s="8"/>
     </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="17"/>
+    </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2564,25 +2748,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.67188" style="9" customWidth="1"/>
-    <col min="2" max="2" width="32.6719" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.1719" style="9" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="9" customWidth="1"/>
-    <col min="5" max="5" width="2.67188" style="9" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="9" customWidth="1"/>
-    <col min="7" max="7" width="25.5" style="9" customWidth="1"/>
-    <col min="8" max="8" width="32.6719" style="9" customWidth="1"/>
-    <col min="9" max="9" width="8.35156" style="9" customWidth="1"/>
-    <col min="10" max="10" width="14.8516" style="9" customWidth="1"/>
-    <col min="11" max="11" width="14.6719" style="9" customWidth="1"/>
-    <col min="12" max="12" width="15.1719" style="9" customWidth="1"/>
-    <col min="13" max="256" width="8.85156" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.67188" style="18" customWidth="1"/>
+    <col min="2" max="2" width="32.6719" style="18" customWidth="1"/>
+    <col min="3" max="3" width="18.1719" style="18" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="2.67188" style="18" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="18" customWidth="1"/>
+    <col min="7" max="7" width="25.5" style="18" customWidth="1"/>
+    <col min="8" max="8" width="32.6719" style="18" customWidth="1"/>
+    <col min="9" max="9" width="8.35156" style="18" customWidth="1"/>
+    <col min="10" max="10" width="14.8516" style="18" customWidth="1"/>
+    <col min="11" max="11" width="14.6719" style="18" customWidth="1"/>
+    <col min="12" max="12" width="15.1719" style="18" customWidth="1"/>
+    <col min="13" max="256" width="8.85156" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -2633,8 +2817,8 @@
       <c r="C2" t="s" s="4">
         <v>45</v>
       </c>
-      <c r="D2" s="10">
-        <v>42136</v>
+      <c r="D2" t="s" s="4">
+        <v>14</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="5">
@@ -2669,8 +2853,8 @@
       <c r="C3" t="s" s="7">
         <v>45</v>
       </c>
-      <c r="D3" s="11">
-        <v>42137</v>
+      <c r="D3" t="s" s="7">
+        <v>23</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="8">
@@ -2694,6 +2878,104 @@
       <c r="L3" t="s" s="7">
         <v>52</v>
       </c>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="11"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="14"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="14"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="14"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
@@ -2706,33 +2988,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.17188" style="12" customWidth="1"/>
-    <col min="2" max="2" width="32.6719" style="12" customWidth="1"/>
-    <col min="3" max="3" width="4.35156" style="12" customWidth="1"/>
-    <col min="4" max="4" width="19.1719" style="12" customWidth="1"/>
-    <col min="5" max="5" width="6.17188" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16" style="12" customWidth="1"/>
-    <col min="7" max="7" width="25.8516" style="12" customWidth="1"/>
-    <col min="8" max="8" width="19.1719" style="12" customWidth="1"/>
-    <col min="9" max="9" width="8.67188" style="12" customWidth="1"/>
-    <col min="10" max="10" width="8.35156" style="12" customWidth="1"/>
-    <col min="11" max="11" width="31.3516" style="12" customWidth="1"/>
-    <col min="12" max="12" width="25.3516" style="12" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="12" customWidth="1"/>
-    <col min="14" max="14" width="11.6719" style="12" customWidth="1"/>
-    <col min="15" max="15" width="32.1719" style="12" customWidth="1"/>
-    <col min="16" max="16" width="25.8516" style="12" customWidth="1"/>
-    <col min="17" max="17" width="10.1719" style="12" customWidth="1"/>
-    <col min="18" max="18" width="32.6719" style="12" customWidth="1"/>
-    <col min="19" max="19" width="7.5" style="12" customWidth="1"/>
-    <col min="20" max="20" width="8.67188" style="12" customWidth="1"/>
-    <col min="21" max="256" width="8.85156" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.17188" style="19" customWidth="1"/>
+    <col min="2" max="2" width="32.6719" style="19" customWidth="1"/>
+    <col min="3" max="3" width="4.35156" style="19" customWidth="1"/>
+    <col min="4" max="4" width="19.1719" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.17188" style="19" customWidth="1"/>
+    <col min="6" max="6" width="16" style="19" customWidth="1"/>
+    <col min="7" max="7" width="25.8516" style="19" customWidth="1"/>
+    <col min="8" max="8" width="19.1719" style="19" customWidth="1"/>
+    <col min="9" max="9" width="8.67188" style="19" customWidth="1"/>
+    <col min="10" max="10" width="8.35156" style="19" customWidth="1"/>
+    <col min="11" max="11" width="31.3516" style="19" customWidth="1"/>
+    <col min="12" max="12" width="25.3516" style="19" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="19" customWidth="1"/>
+    <col min="14" max="14" width="11.6719" style="19" customWidth="1"/>
+    <col min="15" max="15" width="32.1719" style="19" customWidth="1"/>
+    <col min="16" max="16" width="25.8516" style="19" customWidth="1"/>
+    <col min="17" max="17" width="10.1719" style="19" customWidth="1"/>
+    <col min="18" max="18" width="32.6719" style="19" customWidth="1"/>
+    <col min="19" max="19" width="7.5" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.67188" style="19" customWidth="1"/>
+    <col min="21" max="256" width="8.85156" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -2859,7 +3141,7 @@
         <v>79</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="13">
+      <c r="D3" s="20">
         <v>42370</v>
       </c>
       <c r="E3" s="6"/>
@@ -2890,6 +3172,160 @@
       <c r="T3" t="s" s="7">
         <v>78</v>
       </c>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="11"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="14"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="14"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="14"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="14"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="14"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
@@ -2902,34 +3338,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.17188" style="14" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="14" customWidth="1"/>
-    <col min="3" max="3" width="4.35156" style="14" customWidth="1"/>
-    <col min="4" max="4" width="19.1719" style="14" customWidth="1"/>
-    <col min="5" max="5" width="6.17188" style="14" customWidth="1"/>
-    <col min="6" max="6" width="15.1719" style="14" customWidth="1"/>
-    <col min="7" max="7" width="25.8516" style="14" customWidth="1"/>
-    <col min="8" max="8" width="9.17188" style="14" customWidth="1"/>
-    <col min="9" max="9" width="31.3516" style="14" customWidth="1"/>
-    <col min="10" max="10" width="25.3516" style="14" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="14" customWidth="1"/>
-    <col min="12" max="12" width="11.6719" style="14" customWidth="1"/>
-    <col min="13" max="13" width="31.3516" style="14" customWidth="1"/>
-    <col min="14" max="14" width="25.8516" style="14" customWidth="1"/>
-    <col min="15" max="15" width="10.1719" style="14" customWidth="1"/>
-    <col min="16" max="16" width="31.8516" style="14" customWidth="1"/>
-    <col min="17" max="17" width="7.5" style="14" customWidth="1"/>
-    <col min="18" max="18" width="31.6719" style="14" customWidth="1"/>
-    <col min="19" max="19" width="14.6719" style="14" customWidth="1"/>
-    <col min="20" max="20" width="8.67188" style="14" customWidth="1"/>
-    <col min="21" max="21" width="15.1719" style="14" customWidth="1"/>
-    <col min="22" max="256" width="8.85156" style="14" customWidth="1"/>
+    <col min="1" max="1" width="8.17188" style="21" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="4.35156" style="21" customWidth="1"/>
+    <col min="4" max="4" width="19.1719" style="21" customWidth="1"/>
+    <col min="5" max="5" width="6.17188" style="21" customWidth="1"/>
+    <col min="6" max="6" width="15.1719" style="21" customWidth="1"/>
+    <col min="7" max="7" width="25.8516" style="21" customWidth="1"/>
+    <col min="8" max="8" width="9.17188" style="21" customWidth="1"/>
+    <col min="9" max="9" width="31.3516" style="21" customWidth="1"/>
+    <col min="10" max="10" width="25.3516" style="21" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="21" customWidth="1"/>
+    <col min="12" max="12" width="11.6719" style="21" customWidth="1"/>
+    <col min="13" max="13" width="31.3516" style="21" customWidth="1"/>
+    <col min="14" max="14" width="25.8516" style="21" customWidth="1"/>
+    <col min="15" max="15" width="10.1719" style="21" customWidth="1"/>
+    <col min="16" max="16" width="31.8516" style="21" customWidth="1"/>
+    <col min="17" max="17" width="7.5" style="21" customWidth="1"/>
+    <col min="18" max="18" width="31.6719" style="21" customWidth="1"/>
+    <col min="19" max="19" width="14.6719" style="21" customWidth="1"/>
+    <col min="20" max="20" width="8.67188" style="21" customWidth="1"/>
+    <col min="21" max="21" width="15.1719" style="21" customWidth="1"/>
+    <col min="22" max="256" width="8.85156" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -3300,7 +3736,7 @@
         <v>110</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="13">
+      <c r="D7" s="20">
         <v>42370</v>
       </c>
       <c r="E7" s="6"/>
@@ -3328,6 +3764,75 @@
       <c r="U7" t="s" s="7">
         <v>92</v>
       </c>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="11"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="14"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
@@ -3346,35 +3851,35 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.17188" style="15" customWidth="1"/>
-    <col min="2" max="2" width="33.5" style="15" customWidth="1"/>
-    <col min="3" max="3" width="4.35156" style="15" customWidth="1"/>
-    <col min="4" max="4" width="19.1719" style="15" customWidth="1"/>
-    <col min="5" max="5" width="6.17188" style="15" customWidth="1"/>
-    <col min="6" max="6" width="21.6719" style="15" customWidth="1"/>
-    <col min="7" max="7" width="25.8516" style="15" customWidth="1"/>
-    <col min="8" max="8" width="31.3516" style="15" customWidth="1"/>
-    <col min="9" max="9" width="25.3516" style="15" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="15" customWidth="1"/>
-    <col min="11" max="11" width="11.6719" style="15" customWidth="1"/>
-    <col min="12" max="12" width="31.3516" style="15" customWidth="1"/>
-    <col min="13" max="13" width="25.8516" style="15" customWidth="1"/>
-    <col min="14" max="14" width="10.1719" style="15" customWidth="1"/>
-    <col min="15" max="15" width="31.8516" style="15" customWidth="1"/>
-    <col min="16" max="16" width="7.5" style="15" customWidth="1"/>
-    <col min="17" max="17" width="8.67188" style="15" customWidth="1"/>
-    <col min="18" max="18" width="32.5" style="15" customWidth="1"/>
-    <col min="19" max="19" width="13.8516" style="15" customWidth="1"/>
-    <col min="20" max="20" width="8.67188" style="15" customWidth="1"/>
-    <col min="21" max="21" width="6.5" style="15" customWidth="1"/>
-    <col min="22" max="22" width="48" style="15" customWidth="1"/>
-    <col min="23" max="23" width="3.85156" style="15" customWidth="1"/>
-    <col min="24" max="24" width="32.1719" style="15" customWidth="1"/>
-    <col min="25" max="25" width="17.3516" style="15" customWidth="1"/>
-    <col min="26" max="26" width="12.1719" style="15" customWidth="1"/>
-    <col min="27" max="27" width="9" style="15" customWidth="1"/>
-    <col min="28" max="28" width="12.6719" style="15" customWidth="1"/>
-    <col min="29" max="256" width="8.85156" style="15" customWidth="1"/>
+    <col min="1" max="1" width="8.17188" style="22" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="22" customWidth="1"/>
+    <col min="3" max="3" width="4.35156" style="22" customWidth="1"/>
+    <col min="4" max="4" width="19.1719" style="22" customWidth="1"/>
+    <col min="5" max="5" width="6.17188" style="22" customWidth="1"/>
+    <col min="6" max="6" width="21.6719" style="22" customWidth="1"/>
+    <col min="7" max="7" width="25.8516" style="22" customWidth="1"/>
+    <col min="8" max="8" width="31.3516" style="22" customWidth="1"/>
+    <col min="9" max="9" width="25.3516" style="22" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="22" customWidth="1"/>
+    <col min="11" max="11" width="11.6719" style="22" customWidth="1"/>
+    <col min="12" max="12" width="31.3516" style="22" customWidth="1"/>
+    <col min="13" max="13" width="25.8516" style="22" customWidth="1"/>
+    <col min="14" max="14" width="10.1719" style="22" customWidth="1"/>
+    <col min="15" max="15" width="31.8516" style="22" customWidth="1"/>
+    <col min="16" max="16" width="7.5" style="22" customWidth="1"/>
+    <col min="17" max="17" width="8.67188" style="22" customWidth="1"/>
+    <col min="18" max="18" width="32.5" style="22" customWidth="1"/>
+    <col min="19" max="19" width="13.8516" style="22" customWidth="1"/>
+    <col min="20" max="20" width="8.67188" style="22" customWidth="1"/>
+    <col min="21" max="21" width="6.5" style="22" customWidth="1"/>
+    <col min="22" max="22" width="48" style="22" customWidth="1"/>
+    <col min="23" max="23" width="3.85156" style="22" customWidth="1"/>
+    <col min="24" max="24" width="32.1719" style="22" customWidth="1"/>
+    <col min="25" max="25" width="17.3516" style="22" customWidth="1"/>
+    <col min="26" max="26" width="12.1719" style="22" customWidth="1"/>
+    <col min="27" max="27" width="9" style="22" customWidth="1"/>
+    <col min="28" max="28" width="12.6719" style="22" customWidth="1"/>
+    <col min="29" max="256" width="8.85156" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -7371,7 +7876,7 @@
         <v>309</v>
       </c>
       <c r="C60" s="6"/>
-      <c r="D60" s="13">
+      <c r="D60" s="20">
         <v>42370</v>
       </c>
       <c r="E60" s="6"/>
@@ -7415,7 +7920,7 @@
         <v>310</v>
       </c>
       <c r="C61" s="6"/>
-      <c r="D61" s="13">
+      <c r="D61" s="20">
         <v>42370</v>
       </c>
       <c r="E61" s="6"/>
@@ -7462,31 +7967,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.17188" style="16" customWidth="1"/>
-    <col min="2" max="2" width="33.8516" style="16" customWidth="1"/>
-    <col min="3" max="3" width="4.35156" style="16" customWidth="1"/>
-    <col min="4" max="4" width="19.1719" style="16" customWidth="1"/>
-    <col min="5" max="5" width="6.17188" style="16" customWidth="1"/>
-    <col min="6" max="6" width="15.1719" style="16" customWidth="1"/>
-    <col min="7" max="7" width="17.3516" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.3516" style="16" customWidth="1"/>
-    <col min="9" max="9" width="12.6719" style="16" customWidth="1"/>
-    <col min="10" max="10" width="18" style="16" customWidth="1"/>
-    <col min="11" max="11" width="32.8516" style="16" customWidth="1"/>
-    <col min="12" max="12" width="25.3516" style="16" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="16" customWidth="1"/>
-    <col min="14" max="14" width="32.6719" style="16" customWidth="1"/>
-    <col min="15" max="15" width="14.1719" style="16" customWidth="1"/>
-    <col min="16" max="16" width="19.6719" style="16" customWidth="1"/>
-    <col min="17" max="17" width="23.3516" style="16" customWidth="1"/>
-    <col min="18" max="18" width="8.17188" style="16" customWidth="1"/>
-    <col min="19" max="256" width="8.85156" style="16" customWidth="1"/>
+    <col min="1" max="1" width="8.17188" style="23" customWidth="1"/>
+    <col min="2" max="2" width="33.8516" style="23" customWidth="1"/>
+    <col min="3" max="3" width="4.35156" style="23" customWidth="1"/>
+    <col min="4" max="4" width="19.1719" style="23" customWidth="1"/>
+    <col min="5" max="5" width="6.17188" style="23" customWidth="1"/>
+    <col min="6" max="6" width="15.1719" style="23" customWidth="1"/>
+    <col min="7" max="7" width="17.3516" style="23" customWidth="1"/>
+    <col min="8" max="8" width="12.3516" style="23" customWidth="1"/>
+    <col min="9" max="9" width="12.6719" style="23" customWidth="1"/>
+    <col min="10" max="10" width="18" style="23" customWidth="1"/>
+    <col min="11" max="11" width="32.8516" style="23" customWidth="1"/>
+    <col min="12" max="12" width="25.3516" style="23" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="23" customWidth="1"/>
+    <col min="14" max="14" width="32.6719" style="23" customWidth="1"/>
+    <col min="15" max="15" width="14.1719" style="23" customWidth="1"/>
+    <col min="16" max="16" width="19.6719" style="23" customWidth="1"/>
+    <col min="17" max="17" width="23.3516" style="23" customWidth="1"/>
+    <col min="18" max="18" width="8.17188" style="23" customWidth="1"/>
+    <col min="19" max="256" width="8.85156" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -7592,6 +8097,166 @@
       <c r="R2" t="s" s="4">
         <v>21</v>
       </c>
+    </row>
+    <row r="3" ht="13.55" customHeight="1">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="11"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="14"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="14"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="14"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="14"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
@@ -7604,27 +8269,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.17188" style="17" customWidth="1"/>
-    <col min="2" max="2" width="32.6719" style="17" customWidth="1"/>
-    <col min="3" max="3" width="4.35156" style="17" customWidth="1"/>
-    <col min="4" max="4" width="19.1719" style="17" customWidth="1"/>
-    <col min="5" max="5" width="6.17188" style="17" customWidth="1"/>
-    <col min="6" max="6" width="15.1719" style="17" customWidth="1"/>
-    <col min="7" max="7" width="17.3516" style="17" customWidth="1"/>
-    <col min="8" max="8" width="32.8516" style="17" customWidth="1"/>
-    <col min="9" max="9" width="25.3516" style="17" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="17" customWidth="1"/>
-    <col min="11" max="11" width="9.67188" style="17" customWidth="1"/>
-    <col min="12" max="12" width="8.17188" style="17" customWidth="1"/>
-    <col min="13" max="13" width="9.17188" style="17" customWidth="1"/>
-    <col min="14" max="14" width="13.1719" style="17" customWidth="1"/>
-    <col min="15" max="256" width="8.85156" style="17" customWidth="1"/>
+    <col min="1" max="1" width="8.17188" style="24" customWidth="1"/>
+    <col min="2" max="2" width="32.6719" style="24" customWidth="1"/>
+    <col min="3" max="3" width="4.35156" style="24" customWidth="1"/>
+    <col min="4" max="4" width="19.1719" style="24" customWidth="1"/>
+    <col min="5" max="5" width="6.17188" style="24" customWidth="1"/>
+    <col min="6" max="6" width="15.1719" style="24" customWidth="1"/>
+    <col min="7" max="7" width="17.3516" style="24" customWidth="1"/>
+    <col min="8" max="8" width="32.8516" style="24" customWidth="1"/>
+    <col min="9" max="9" width="25.3516" style="24" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="24" customWidth="1"/>
+    <col min="11" max="11" width="9.67188" style="24" customWidth="1"/>
+    <col min="12" max="12" width="8.17188" style="24" customWidth="1"/>
+    <col min="13" max="13" width="9.17188" style="24" customWidth="1"/>
+    <col min="14" max="14" width="13.1719" style="24" customWidth="1"/>
+    <col min="15" max="256" width="8.85156" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -7746,6 +8411,118 @@
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
+    </row>
+    <row r="4" ht="13.55" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="14"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="14"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="14"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>
@@ -7758,29 +8535,29 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.17188" style="18" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="18" customWidth="1"/>
-    <col min="3" max="3" width="14.7734" style="18" customWidth="1"/>
-    <col min="4" max="4" width="19.1719" style="18" customWidth="1"/>
-    <col min="5" max="5" width="9.67188" style="18" customWidth="1"/>
-    <col min="6" max="6" width="15.1719" style="18" customWidth="1"/>
-    <col min="7" max="7" width="14.1719" style="18" customWidth="1"/>
-    <col min="8" max="8" width="32.8516" style="18" customWidth="1"/>
-    <col min="9" max="9" width="13.3516" style="18" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="18" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="18" customWidth="1"/>
-    <col min="12" max="12" width="8.17188" style="18" customWidth="1"/>
-    <col min="13" max="13" width="29.8516" style="18" customWidth="1"/>
-    <col min="14" max="14" width="31.1719" style="18" customWidth="1"/>
-    <col min="15" max="15" width="32.6719" style="18" customWidth="1"/>
-    <col min="16" max="16" width="8.17188" style="18" customWidth="1"/>
-    <col min="17" max="256" width="8.85156" style="18" customWidth="1"/>
+    <col min="1" max="1" width="8.17188" style="25" customWidth="1"/>
+    <col min="2" max="2" width="32.5" style="25" customWidth="1"/>
+    <col min="3" max="3" width="14.8516" style="25" customWidth="1"/>
+    <col min="4" max="4" width="19.1719" style="25" customWidth="1"/>
+    <col min="5" max="5" width="9.67188" style="25" customWidth="1"/>
+    <col min="6" max="6" width="15.1719" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14.1719" style="25" customWidth="1"/>
+    <col min="8" max="8" width="32.8516" style="25" customWidth="1"/>
+    <col min="9" max="9" width="13.3516" style="25" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="25" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="25" customWidth="1"/>
+    <col min="12" max="12" width="8.17188" style="25" customWidth="1"/>
+    <col min="13" max="13" width="29.8516" style="25" customWidth="1"/>
+    <col min="14" max="14" width="31.1719" style="25" customWidth="1"/>
+    <col min="15" max="15" width="32.6719" style="25" customWidth="1"/>
+    <col min="16" max="16" width="8.17188" style="25" customWidth="1"/>
+    <col min="17" max="256" width="8.85156" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.1" customHeight="1">
@@ -7790,7 +8567,7 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="19">
+      <c r="C1" t="s" s="26">
         <v>2</v>
       </c>
       <c r="D1" t="s" s="2">
@@ -7840,8 +8617,8 @@
       <c r="B2" t="s" s="4">
         <v>340</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21">
+      <c r="C2" s="27"/>
+      <c r="D2" s="28">
         <v>42370</v>
       </c>
       <c r="E2" s="3"/>
@@ -7882,8 +8659,8 @@
       <c r="B3" t="s" s="7">
         <v>346</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="13">
+      <c r="C3" s="29"/>
+      <c r="D3" s="20">
         <v>42370</v>
       </c>
       <c r="E3" s="6"/>
@@ -7922,7 +8699,7 @@
       <c r="B4" t="s" s="7">
         <v>350</v>
       </c>
-      <c r="C4" t="s" s="23">
+      <c r="C4" t="s" s="30">
         <v>351</v>
       </c>
       <c r="D4" t="s" s="7">
@@ -7956,7 +8733,7 @@
       <c r="B5" t="s" s="7">
         <v>353</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="29"/>
       <c r="D5" t="s" s="7">
         <v>354</v>
       </c>
@@ -7979,7 +8756,7 @@
       <c r="K5" t="s" s="7">
         <v>357</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="31">
         <v>33369696</v>
       </c>
       <c r="M5" s="6"/>
@@ -7998,7 +8775,7 @@
       <c r="B6" t="s" s="7">
         <v>52</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="29"/>
       <c r="D6" t="s" s="7">
         <v>330</v>
       </c>
@@ -8021,7 +8798,7 @@
       <c r="K6" t="s" s="7">
         <v>361</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="31">
         <v>33369696</v>
       </c>
       <c r="M6" s="6"/>
@@ -8035,43 +8812,59 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" ht="12.9" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" t="s" s="7">
-        <v>362</v>
-      </c>
-      <c r="C7" t="s" s="23">
-        <v>363</v>
-      </c>
-      <c r="D7" t="s" s="7">
-        <v>330</v>
-      </c>
-      <c r="E7" s="11">
-        <v>41858</v>
-      </c>
-      <c r="F7" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="G7" t="s" s="7">
-        <v>355</v>
-      </c>
-      <c r="H7" t="s" s="7">
-        <v>164</v>
-      </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" t="s" s="7">
-        <v>350</v>
-      </c>
-      <c r="O7" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="P7" t="s" s="7">
-        <v>364</v>
-      </c>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="11"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="14"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0.511806" footer="0.511806"/>

</xml_diff>

<commit_message>
treat CPR numbers as strings internally, and only accept 10-digit numbers
...and fix an error where we actually output 12-digit CPR numbers :(
</commit_message>
<xml_diff>
--- a/tests/fixtures/MAGENTA_01.xlsx
+++ b/tests/fixtures/MAGENTA_01.xlsx
@@ -2574,7 +2574,7 @@
         <v>21</v>
       </c>
       <c r="M2" s="5">
-        <v>10119001010</v>
+        <v>101001010</v>
       </c>
     </row>
     <row r="3" ht="12.9" customHeight="1">
@@ -2611,7 +2611,7 @@
         <v>21</v>
       </c>
       <c r="M3" s="8">
-        <v>101120101010</v>
+        <v>1011101010</v>
       </c>
     </row>
     <row r="4" ht="12.9" customHeight="1">

</xml_diff>